<commit_message>
Commit Data + Controllers
</commit_message>
<xml_diff>
--- a/VacationAccountingSystem/examples/departments.xlsx
+++ b/VacationAccountingSystem/examples/departments.xlsx
@@ -20,24 +20,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t xml:space="preserve">id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">parentId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Отдел 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Отдел 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Отдел 1.1</t>
+    <t xml:space="preserve">parentName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Отдел продаж</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT-отдел</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Финансово-экономический департамент</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Бухгалтерия</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Юридический отдел</t>
   </si>
 </sst>
 </file>
@@ -247,13 +250,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.56"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -262,35 +269,36 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>1</v>
+      <c r="B5" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>